<commit_message>
Commit 8 - Major Change
</commit_message>
<xml_diff>
--- a/input/input.xlsx
+++ b/input/input.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LoginLogout" sheetId="1" r:id="rId1"/>
     <sheet name="MultipleLogin" sheetId="2" r:id="rId2"/>
     <sheet name="DataBase" sheetId="3" r:id="rId3"/>
+    <sheet name="AddEmployee" sheetId="4" r:id="rId4"/>
+    <sheet name="NewUser" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>USER NAME</t>
   </si>
@@ -46,6 +48,15 @@
   </si>
   <si>
     <t>Kumar</t>
+  </si>
+  <si>
+    <t>user7</t>
+  </si>
+  <si>
+    <t>Karan</t>
+  </si>
+  <si>
+    <t>Arjun</t>
   </si>
 </sst>
 </file>
@@ -398,7 +409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -501,4 +512,78 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>